<commit_message>
small overhaul and upgrade to 4.6
</commit_message>
<xml_diff>
--- a/.doc/XLSX/Data.xlsx
+++ b/.doc/XLSX/Data.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Items" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -27,33 +27,9 @@
     <t>description</t>
   </si>
   <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>percentage</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>sequence</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>json</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -63,35 +39,29 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>Sequence</t>
-  </si>
-  <si>
-    <t>foo_0</t>
-  </si>
-  <si>
-    <t>Foo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test data for csv importer</t>
-  </si>
-  <si>
-    <t>[1,2,3]</t>
+    <t>herb_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Healing Herb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herbs used to cure wound.</t>
+  </si>
+  <si>
+    <t>potion_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potion Of Healing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instantly recover health points</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="11">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -99,18 +69,115 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.000000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color indexed="2"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.000000"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <color theme="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+        <bgColor indexed="47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -118,22 +185,132 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="14">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf fontId="1" fillId="3" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="4" borderId="2" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="3" fillId="4" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="4" fillId="2" borderId="3" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
+    <xf fontId="0" fillId="5" borderId="4" numFmtId="0" applyNumberFormat="0" applyFont="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="5" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
+    <xf fontId="6" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
+    <xf fontId="7" fillId="6" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="8" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="9" fillId="8" borderId="5" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+    <xf fontId="10" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="14">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Currency [0]" xfId="2" builtinId="7"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="6" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="7" builtinId="24"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Explanatory Text" xfId="10" builtinId="53"/>
+    <cellStyle name="Bad" xfId="11" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="12" builtinId="28"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -146,22 +323,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="表格1" ref="A3:G4">
-  <autoFilter ref="A3:G4"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="id"/>
-    <tableColumn id="2" name="Name"/>
-    <tableColumn id="3" name="description"/>
-    <tableColumn id="4" name="Rank"/>
-    <tableColumn id="5" name="Hit Rate"/>
-    <tableColumn id="6" name="boolean"/>
-    <tableColumn id="7" name="Damage"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,125 +818,94 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="5.7421875"/>
-    <col bestFit="1" min="2" max="2" width="8.25390625"/>
-    <col bestFit="1" min="3" max="3" width="22.65234375"/>
-    <col bestFit="1" min="4" max="4" width="7.68359375"/>
-    <col bestFit="1" min="5" max="5" width="12.94140625"/>
-    <col bestFit="1" min="6" max="6" width="10.3125"/>
-    <col bestFit="1" min="7" max="7" width="11.57421875"/>
+    <col bestFit="1" min="2" max="2" width="15.68359375"/>
+    <col bestFit="1" min="3" max="3" width="26.7734375"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.10000000000000001</v>
-      </c>
-      <c r="F4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="5" ht="14.25"/>
-    <row r="6" ht="14.25"/>
-    <row r="7" ht="14.25"/>
-    <row r="8" ht="14.25"/>
-    <row r="9" ht="14.25"/>
+    <row r="5" ht="14.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>